<commit_message>
Add events BeforeNumbersRenderMethodName and AfterNumbersRenderMethodName into DynamicPanel
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
@@ -68,7 +68,7 @@
     <x:numFmt numFmtId="166" formatCode="#,0.0"/>
     <x:numFmt numFmtId="167" formatCode="$ #,0.00"/>
   </x:numFmts>
-  <x:fonts count="4">
+  <x:fonts count="5">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -81,6 +81,13 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFFFFFF"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -101,12 +108,18 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="3">
+  <x:fills count="4">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF808080"/>
+        <x:bgColor rgb="FF808080"/>
+      </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
@@ -134,11 +147,11 @@
       </x:diagonal>
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
+      <x:left style="medium">
+        <x:color rgb="FFFF0000"/>
       </x:left>
-      <x:right style="medium">
-        <x:color rgb="FFFF0000"/>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
       </x:right>
       <x:top style="medium">
         <x:color rgb="FFFF0000"/>
@@ -151,8 +164,8 @@
       </x:diagonal>
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="medium">
-        <x:color rgb="FFFF0000"/>
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
       </x:left>
       <x:right style="none">
         <x:color rgb="FF000000"/>
@@ -171,8 +184,8 @@
       <x:left style="none">
         <x:color rgb="FF000000"/>
       </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
+      <x:right style="medium">
+        <x:color rgb="FFFF0000"/>
       </x:right>
       <x:top style="medium">
         <x:color rgb="FFFF0000"/>
@@ -202,6 +215,40 @@
       </x:diagonal>
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="dashed">
+        <x:color rgb="FF008000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="dashed">
+        <x:color rgb="FF008000"/>
+      </x:top>
+      <x:bottom style="dashed">
+        <x:color rgb="FF008000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="dashed">
+        <x:color rgb="FF008000"/>
+      </x:top>
+      <x:bottom style="dashed">
+        <x:color rgb="FF008000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
       </x:left>
@@ -218,42 +265,8 @@
         <x:color rgb="FF000000"/>
       </x:diagonal>
     </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="dashed">
-        <x:color rgb="FF008000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="dashed">
-        <x:color rgb="FF008000"/>
-      </x:top>
-      <x:bottom style="dashed">
-        <x:color rgb="FF008000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="dashed">
-        <x:color rgb="FF008000"/>
-      </x:top>
-      <x:bottom style="dashed">
-        <x:color rgb="FF008000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -266,29 +279,32 @@
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="166" fontId="2" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="167" fontId="3" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="167" fontId="4" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -305,31 +321,35 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -628,7 +648,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:T6"/>
+  <x:dimension ref="A1:Z7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -641,102 +661,125 @@
     <x:col min="8" max="8" width="20.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:20">
-      <x:c r="B2" s="2" t="s">
+    <x:row r="2" spans="1:26">
+      <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="C2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D2" s="3" t="s">
+      <x:c r="D2" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E2" s="3" t="s">
+      <x:c r="E2" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="F2" s="3" t="s">
+      <x:c r="F2" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="G2" s="3" t="s">
+      <x:c r="G2" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="H2" s="1" t="s">
+      <x:c r="H2" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:20">
+    <x:row r="3" spans="1:26">
       <x:c r="B3" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="4" t="s">
+      <x:c r="C3" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D3" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E3" s="4" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F3" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G3" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H3" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D3" s="4" t="s">
+    </x:row>
+    <x:row r="4" spans="1:26">
+      <x:c r="B4" s="7" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="7" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D4" s="7" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E3" s="4" t="s"/>
-      <x:c r="F3" s="4" t="s"/>
-      <x:c r="G3" s="6" t="n">
+      <x:c r="E4" s="7" t="s"/>
+      <x:c r="F4" s="7" t="s"/>
+      <x:c r="G4" s="6" t="n">
         <x:v>523635.93</x:v>
       </x:c>
-      <x:c r="H3" s="5" t="n">
+      <x:c r="H4" s="5" t="n">
         <x:v>2.6</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:20">
-      <x:c r="B4" s="4" t="n">
+    <x:row r="5" spans="1:26">
+      <x:c r="B5" s="7" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C4" s="4" t="s">
+      <x:c r="C5" s="7" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D4" s="4" t="s">
+      <x:c r="D5" s="7" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E4" s="4" t="n">
+      <x:c r="E5" s="7" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F4" s="4" t="s">
+      <x:c r="F5" s="7" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G4" s="6" t="s"/>
-      <x:c r="H4" s="5" t="n">
+      <x:c r="G5" s="6" t="s"/>
+      <x:c r="H5" s="5" t="n">
         <x:v>5.2</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:20">
-      <x:c r="B5" s="4" t="n">
+    <x:row r="6" spans="1:26">
+      <x:c r="B6" s="7" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C5" s="4" t="s">
+      <x:c r="C6" s="7" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D5" s="4" t="s"/>
-      <x:c r="E5" s="4" t="s"/>
-      <x:c r="F5" s="4" t="s">
+      <x:c r="D6" s="7" t="s"/>
+      <x:c r="E6" s="7" t="s"/>
+      <x:c r="F6" s="7" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="G5" s="6" t="n">
+      <x:c r="G6" s="6" t="n">
         <x:v>100000.5532</x:v>
       </x:c>
-      <x:c r="H5" s="5" t="n">
+      <x:c r="H6" s="5" t="n">
         <x:v>7.8</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:20">
-      <x:c r="B6" s="8" t="n">
+    <x:row r="7" spans="1:26">
+      <x:c r="B7" s="8" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C6" s="9" t="n">
+      <x:c r="C7" s="9" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D6" s="9" t="s"/>
-      <x:c r="E6" s="9" t="s"/>
-      <x:c r="F6" s="9" t="s"/>
-      <x:c r="G6" s="10" t="n">
+      <x:c r="D7" s="9" t="s"/>
+      <x:c r="E7" s="9" t="s"/>
+      <x:c r="F7" s="9" t="s"/>
+      <x:c r="G7" s="10" t="n">
         <x:v>623636.4832</x:v>
       </x:c>
-      <x:c r="H6" s="7" t="n">
+      <x:c r="H7" s="11" t="n">
         <x:v>15.6</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Support result range grouping in dynamic panel
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <x:si>
+    <x:t>Stub</x:t>
+  </x:si>
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -648,7 +651,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:Z7"/>
+  <x:dimension ref="A1:Z8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -661,27 +664,32 @@
     <x:col min="8" max="8" width="20.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
+    <x:row r="1" spans="1:26">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
     <x:row r="2" spans="1:26">
       <x:c r="B2" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F2" s="2" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G2" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:26">
@@ -712,10 +720,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C4" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D4" s="7" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="7" t="s"/>
       <x:c r="F4" s="7" t="s"/>
@@ -731,16 +739,16 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C5" s="7" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D5" s="7" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E5" s="7" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="F5" s="7" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G5" s="6" t="s"/>
       <x:c r="H5" s="5" t="n">
@@ -752,12 +760,14 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C6" s="7" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D6" s="7" t="s"/>
-      <x:c r="E6" s="7" t="s"/>
+      <x:c r="E6" s="7" t="n">
+        <x:v>1</x:v>
+      </x:c>
       <x:c r="F6" s="7" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G6" s="6" t="n">
         <x:v>100000.5532</x:v>
@@ -783,7 +793,18 @@
         <x:v>15.6</x:v>
       </x:c>
     </x:row>
+    <x:row r="8" spans="1:26">
+      <x:c r="I8" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
+  <x:mergeCells count="4">
+    <x:mergeCell ref="E4:E4"/>
+    <x:mergeCell ref="E5:E6"/>
+    <x:mergeCell ref="A1:A1"/>
+    <x:mergeCell ref="I8:I8"/>
+  </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
Support for ClosedXml 0.94
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <x:si>
-    <x:t>Stub</x:t>
-  </x:si>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -67,8 +64,8 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="4">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="#,0.00"/>
-    <x:numFmt numFmtId="166" formatCode="#,0.0"/>
+    <x:numFmt numFmtId="165" formatCode="#,0.0"/>
+    <x:numFmt numFmtId="166" formatCode="#,0.00"/>
     <x:numFmt numFmtId="167" formatCode="$ #,0.00"/>
   </x:numFmts>
   <x:fonts count="5">
@@ -121,13 +118,11 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF808080"/>
-        <x:bgColor rgb="FF808080"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF00DDDD"/>
-        <x:bgColor rgb="FF00DDDD"/>
       </x:patternFill>
     </x:fill>
   </x:fills>
@@ -285,15 +280,15 @@
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="166" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -303,7 +298,7 @@
     <x:xf numFmtId="167" fontId="4" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="166" fontId="4" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -328,18 +323,18 @@
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -352,7 +347,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -651,7 +646,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:Z8"/>
+  <x:dimension ref="A1:Z7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -664,32 +659,27 @@
     <x:col min="8" max="8" width="20.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:26">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
     <x:row r="2" spans="1:26">
       <x:c r="B2" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="D2" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="s">
+      <x:c r="E2" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E2" s="2" t="s">
+      <x:c r="F2" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F2" s="2" t="s">
+      <x:c r="G2" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G2" s="2" t="s">
+      <x:c r="H2" s="3" t="s">
         <x:v>6</x:v>
-      </x:c>
-      <x:c r="H2" s="3" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:26">
@@ -716,63 +706,61 @@
       </x:c>
     </x:row>
     <x:row r="4" spans="1:26">
-      <x:c r="B4" s="7" t="n">
+      <x:c r="B4" s="5" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C4" s="7" t="s">
+      <x:c r="C4" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D4" s="5" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D4" s="7" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E4" s="7" t="s"/>
-      <x:c r="F4" s="7" t="s"/>
+      <x:c r="E4" s="5" t="s"/>
+      <x:c r="F4" s="5" t="s"/>
       <x:c r="G4" s="6" t="n">
         <x:v>523635.93</x:v>
       </x:c>
-      <x:c r="H4" s="5" t="n">
+      <x:c r="H4" s="7" t="n">
         <x:v>2.6</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:26">
-      <x:c r="B5" s="7" t="n">
+      <x:c r="B5" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C5" s="7" t="s">
+      <x:c r="C5" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D5" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D5" s="7" t="s">
+      <x:c r="E5" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F5" s="5" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E5" s="7" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F5" s="7" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="G5" s="6" t="s"/>
-      <x:c r="H5" s="5" t="n">
+      <x:c r="H5" s="7" t="n">
         <x:v>5.2</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:26">
-      <x:c r="B6" s="7" t="n">
+      <x:c r="B6" s="5" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C6" s="7" t="s">
+      <x:c r="C6" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="E6" s="5" t="s"/>
+      <x:c r="F6" s="5" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="D6" s="7" t="s"/>
-      <x:c r="E6" s="7" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F6" s="7" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="G6" s="6" t="n">
         <x:v>100000.5532</x:v>
       </x:c>
-      <x:c r="H6" s="5" t="n">
+      <x:c r="H6" s="7" t="n">
         <x:v>7.8</x:v>
       </x:c>
     </x:row>
@@ -793,17 +781,10 @@
         <x:v>15.6</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:26">
-      <x:c r="I8" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
-  <x:mergeCells count="4">
+  <x:mergeCells count="2">
     <x:mergeCell ref="E4:E4"/>
     <x:mergeCell ref="E5:E6"/>
-    <x:mergeCell ref="A1:A1"/>
-    <x:mergeCell ref="I8:I8"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>